<commit_message>
changed bat file, current directory variable
changed bat file, to use current directory variable %~dp0 refers to the full path to the batch file's directory (static)

%~dpnx0 refers to the full path to the batch directory and file name (static).

%cd% refers to the current working directory (variable)
</commit_message>
<xml_diff>
--- a/ASMtemplate.xlsx
+++ b/ASMtemplate.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiaodong\Documents\GitHub\Make-ASM-template-from-Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FC2FDFF5-4E64-4962-8BEB-D068309459D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22488" windowHeight="9420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22485" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -335,19 +341,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -366,55 +368,8 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -422,105 +377,8 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,198 +393,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.0499893185216834"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -752,252 +424,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1015,68 +445,24 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="50">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
-    <cellStyle name="常规 2" xfId="49"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1363,26 +749,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.287037037037" customWidth="1"/>
-    <col min="2" max="2" width="22.712962962963" customWidth="1"/>
-    <col min="3" max="3" width="14.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="16.287037037037" customWidth="1"/>
-    <col min="6" max="6" width="11.7037037037037" customWidth="1"/>
-    <col min="7" max="7" width="9.56481481481481" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1429,100 +815,97 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:14">
       <c r="C2" s="9">
         <v>43206</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:CE16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:CE15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.4259259259259" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.8611111111111" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.42592592592593" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.86111111111111" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1388888888889" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.4259259259259" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.4259259259259" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.8611111111111" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="8" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.8611111111111" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.42592592592593" style="2" customWidth="1"/>
-    <col min="13" max="16" width="9.13888888888889" style="2"/>
-    <col min="17" max="17" width="22.4259259259259" style="2" customWidth="1"/>
-    <col min="18" max="18" width="18.5648148148148" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.13888888888889" style="2"/>
-    <col min="20" max="20" width="31.5648148148148" style="2" customWidth="1"/>
-    <col min="21" max="21" width="12.8611111111111" style="2" customWidth="1"/>
-    <col min="22" max="22" width="9.86111111111111" style="2" customWidth="1"/>
-    <col min="23" max="23" width="9.56481481481481" style="2" customWidth="1"/>
-    <col min="24" max="24" width="9.13888888888889" style="2"/>
-    <col min="25" max="25" width="16.8611111111111" style="2" customWidth="1"/>
-    <col min="26" max="26" width="13.5648148148148" style="2" customWidth="1"/>
-    <col min="27" max="27" width="27.5648148148148" style="2" customWidth="1"/>
-    <col min="28" max="28" width="15.287037037037" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="2" customWidth="1"/>
+    <col min="13" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="22.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="31.5703125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="2"/>
+    <col min="25" max="25" width="16.85546875" style="2" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="27.5703125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="15.28515625" style="2" customWidth="1"/>
     <col min="29" max="29" width="20" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.1388888888889" style="2" customWidth="1"/>
-    <col min="31" max="31" width="12.1388888888889" style="3" customWidth="1"/>
-    <col min="32" max="32" width="15.7037037037037" style="4" customWidth="1"/>
-    <col min="33" max="33" width="15.8611111111111" style="4" customWidth="1"/>
-    <col min="34" max="34" width="13.8611111111111" style="4" customWidth="1"/>
-    <col min="35" max="35" width="18.712962962963" style="4" customWidth="1"/>
-    <col min="36" max="36" width="17.5648148148148" style="5" customWidth="1"/>
-    <col min="37" max="37" width="9.13888888888889" style="3"/>
-    <col min="38" max="41" width="9.13888888888889" style="4"/>
-    <col min="42" max="42" width="9.13888888888889" style="5"/>
-    <col min="43" max="43" width="17.8611111111111" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="12.140625" style="3" customWidth="1"/>
+    <col min="32" max="32" width="15.7109375" style="4" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" style="4" customWidth="1"/>
+    <col min="34" max="34" width="13.85546875" style="4" customWidth="1"/>
+    <col min="35" max="35" width="18.7109375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.5703125" style="5" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="3"/>
+    <col min="38" max="41" width="9.140625" style="4"/>
+    <col min="42" max="42" width="9.140625" style="5"/>
+    <col min="43" max="43" width="17.85546875" style="2" customWidth="1"/>
     <col min="44" max="44" width="17" style="2" customWidth="1"/>
-    <col min="45" max="45" width="19.287037037037" style="2" customWidth="1"/>
-    <col min="46" max="46" width="18.5648148148148" style="2" customWidth="1"/>
-    <col min="47" max="51" width="9.13888888888889" style="2"/>
-    <col min="52" max="52" width="9.13888888888889" style="5"/>
-    <col min="53" max="53" width="15.1388888888889" style="2" customWidth="1"/>
+    <col min="45" max="45" width="19.28515625" style="2" customWidth="1"/>
+    <col min="46" max="46" width="18.5703125" style="2" customWidth="1"/>
+    <col min="47" max="51" width="9.140625" style="2"/>
+    <col min="52" max="52" width="9.140625" style="5"/>
+    <col min="53" max="53" width="15.140625" style="2" customWidth="1"/>
     <col min="54" max="54" width="15" style="2" customWidth="1"/>
     <col min="55" max="55" width="20" style="2" customWidth="1"/>
-    <col min="56" max="63" width="9.13888888888889" style="2"/>
-    <col min="64" max="64" width="14.7037037037037" style="2" customWidth="1"/>
-    <col min="65" max="65" width="15.287037037037" style="2" customWidth="1"/>
-    <col min="66" max="67" width="18.8611111111111" style="6" customWidth="1"/>
-    <col min="68" max="68" width="22.1388888888889" style="6" customWidth="1"/>
-    <col min="69" max="69" width="11.5648148148148" style="6" customWidth="1"/>
-    <col min="70" max="70" width="22.1388888888889" style="6" customWidth="1"/>
-    <col min="71" max="71" width="11.5648148148148" style="6" customWidth="1"/>
-    <col min="72" max="72" width="16.712962962963" style="2" customWidth="1"/>
-    <col min="73" max="73" width="21.5648148148148" style="2" customWidth="1"/>
-    <col min="74" max="74" width="17.712962962963" style="2" customWidth="1"/>
-    <col min="75" max="75" width="16.712962962963" style="2" customWidth="1"/>
-    <col min="76" max="76" width="21.5648148148148" style="2" customWidth="1"/>
-    <col min="77" max="77" width="17.712962962963" style="2" customWidth="1"/>
-    <col min="78" max="78" width="16.712962962963" style="2" customWidth="1"/>
-    <col min="79" max="79" width="21.5648148148148" style="2" customWidth="1"/>
-    <col min="80" max="80" width="17.712962962963" style="2" customWidth="1"/>
-    <col min="81" max="81" width="16.712962962963" style="2" customWidth="1"/>
-    <col min="82" max="82" width="21.5648148148148" style="2" customWidth="1"/>
-    <col min="83" max="83" width="17.712962962963" style="2" customWidth="1"/>
+    <col min="56" max="63" width="9.140625" style="2"/>
+    <col min="64" max="64" width="14.7109375" style="2" customWidth="1"/>
+    <col min="65" max="65" width="15.28515625" style="2" customWidth="1"/>
+    <col min="66" max="67" width="18.85546875" style="6" customWidth="1"/>
+    <col min="68" max="68" width="22.140625" style="6" customWidth="1"/>
+    <col min="69" max="69" width="11.5703125" style="6" customWidth="1"/>
+    <col min="70" max="70" width="22.140625" style="6" customWidth="1"/>
+    <col min="71" max="71" width="11.5703125" style="6" customWidth="1"/>
+    <col min="72" max="72" width="16.7109375" style="2" customWidth="1"/>
+    <col min="73" max="73" width="21.5703125" style="2" customWidth="1"/>
+    <col min="74" max="74" width="17.7109375" style="2" customWidth="1"/>
+    <col min="75" max="75" width="16.7109375" style="2" customWidth="1"/>
+    <col min="76" max="76" width="21.5703125" style="2" customWidth="1"/>
+    <col min="77" max="77" width="17.7109375" style="2" customWidth="1"/>
+    <col min="78" max="78" width="16.7109375" style="2" customWidth="1"/>
+    <col min="79" max="79" width="21.5703125" style="2" customWidth="1"/>
+    <col min="80" max="80" width="17.7109375" style="2" customWidth="1"/>
+    <col min="81" max="81" width="16.7109375" style="2" customWidth="1"/>
+    <col min="82" max="82" width="21.5703125" style="2" customWidth="1"/>
+    <col min="83" max="83" width="17.7109375" style="2" customWidth="1"/>
     <col min="84" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:83">
+    <row r="1" spans="1:83" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1773,7 +1156,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="5:65">
+    <row r="2" spans="1:83">
       <c r="E2" s="2" t="s">
         <v>96</v>
       </c>
@@ -1835,110 +1218,47 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="5:65">
-      <c r="E3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3926909790</v>
-      </c>
-      <c r="H3" s="2">
-        <v>14.5</v>
-      </c>
-      <c r="I3" s="2">
-        <v>100</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="K3" s="2">
-        <v>13.5</v>
-      </c>
-      <c r="M3" s="2">
-        <v>331</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="P3" s="7">
-        <v>331</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>331</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="BB3" s="2">
-        <v>380</v>
-      </c>
-      <c r="BC3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BM3" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="16:16">
+    <row r="3" spans="1:83">
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:83">
       <c r="P4" s="7"/>
     </row>
-    <row r="5" spans="16:16">
+    <row r="5" spans="1:83">
       <c r="P5" s="7"/>
     </row>
-    <row r="6" spans="16:16">
+    <row r="6" spans="1:83">
       <c r="P6" s="7"/>
     </row>
-    <row r="7" spans="16:16">
+    <row r="7" spans="1:83">
       <c r="P7" s="7"/>
     </row>
-    <row r="8" spans="16:16">
+    <row r="8" spans="1:83">
       <c r="P8" s="7"/>
     </row>
-    <row r="9" spans="16:16">
+    <row r="9" spans="1:83">
       <c r="P9" s="7"/>
     </row>
-    <row r="10" spans="16:16">
+    <row r="10" spans="1:83">
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="16:16">
+    <row r="11" spans="1:83">
       <c r="P11" s="7"/>
     </row>
-    <row r="12" spans="16:16">
+    <row r="12" spans="1:83">
       <c r="P12" s="7"/>
     </row>
-    <row r="13" spans="16:16">
+    <row r="13" spans="1:83">
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="16:16">
+    <row r="14" spans="1:83">
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="16:16">
+    <row r="15" spans="1:83">
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="16:16">
-      <c r="P16" s="7"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed GW, changed column mapping according to new invoice/packing template
</commit_message>
<xml_diff>
--- a/ASMtemplate.xlsx
+++ b/ASMtemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiaodong\Documents\GitHub\Make-ASM-template-from-Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\PycharmProjects\Make-ASM-template-from-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FC2FDFF5-4E64-4962-8BEB-D068309459D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA05BDD-3BC5-4D29-B985-869232A05B10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22485" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -445,7 +445,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -832,7 +832,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1166,9 +1166,6 @@
       <c r="G2" s="2">
         <v>3926909790</v>
       </c>
-      <c r="H2" s="2">
-        <v>14.5</v>
-      </c>
       <c r="I2" s="2">
         <v>100</v>
       </c>

</xml_diff>